<commit_message>
ANIM Player combo heavy
</commit_message>
<xml_diff>
--- a/Documents/CombatSystem/ComboSheet.xlsx
+++ b/Documents/CombatSystem/ComboSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eliott SPARWASSER\Desktop\PFA\PFEURA\Documents\CombatSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorian MAGNO\Desktop\PFEURA\Documents\CombatSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C72786B-E50E-4A20-A49E-FEE6DA481156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C427D4E8-21C6-4CFC-9739-B3F781496DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Combo Overview" sheetId="1" r:id="rId1"/>
@@ -670,6 +670,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -678,15 +687,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2188,11 +2188,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
@@ -21619,7 +21619,7 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
@@ -41106,11 +41106,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E005FA2-9999-48D2-8415-3EC36386B2A4}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
@@ -41340,15 +41340,15 @@
       <c r="G10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="45" t="s">
+      <c r="I10" s="50"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="49"/>
       <c r="M10" s="29"/>
       <c r="N10" s="29"/>
       <c r="O10" s="22"/>
@@ -41373,10 +41373,10 @@
       <c r="H11" s="12"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="K11" s="50" t="s">
+      <c r="K11" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="50"/>
+      <c r="L11" s="45"/>
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
       <c r="O11" s="8"/>
@@ -41538,11 +41538,11 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="48" t="s">
+      <c r="H17" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
       <c r="K17" s="44"/>
       <c r="L17" s="44"/>
       <c r="M17" s="35"/>
@@ -60318,6 +60318,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
     <mergeCell ref="A1:O5"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:I7"/>
@@ -60326,21 +60341,6 @@
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:G1000">
     <cfRule type="containsBlanks" dxfId="18" priority="10">

</xml_diff>